<commit_message>
Project Alpha build complete.
</commit_message>
<xml_diff>
--- a/Top20Test.xlsx
+++ b/Top20Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72">
   <si>
     <t>GE Canada</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>user4</t>
-  </si>
-  <si>
-    <t>supppyy</t>
   </si>
   <si>
     <t>522639468</t>
@@ -241,8 +238,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="179" formatCode="[$-10409]&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="[$-10409]#,##0.00;\(#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="[$-10409]&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="[$-10409]#,##0.00;\(#,##0.00\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -255,7 +252,7 @@
       <sz val="23.95"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -263,27 +260,27 @@
       <sz val="11.95"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -438,7 +435,7 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -446,15 +443,15 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="180" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -462,15 +459,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -485,18 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -983,9 +980,9 @@
   </sheetPr>
   <dimension ref="A1:CY29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BI5" sqref="BI5:BK5"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1088,29 +1085,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:103" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13"/>
-      <c r="D1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="A1" s="16"/>
+      <c r="D1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:103" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="D2" s="15" t="s">
+      <c r="A2" s="16"/>
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:103" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="A3" s="16"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1140,109 +1137,109 @@
       <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="17"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="11"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="11"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="15"/>
       <c r="AG4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-      <c r="AV4" s="10"/>
-      <c r="AW4" s="10"/>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="11"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="14"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="14"/>
+      <c r="AP4" s="14"/>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="14"/>
+      <c r="AS4" s="14"/>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="14"/>
+      <c r="AV4" s="14"/>
+      <c r="AW4" s="14"/>
+      <c r="AX4" s="14"/>
+      <c r="AY4" s="14"/>
+      <c r="AZ4" s="15"/>
       <c r="BA4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
-      <c r="BD4" s="10"/>
-      <c r="BE4" s="10"/>
-      <c r="BF4" s="10"/>
-      <c r="BG4" s="10"/>
-      <c r="BH4" s="10"/>
-      <c r="BI4" s="10"/>
-      <c r="BJ4" s="10"/>
-      <c r="BK4" s="10"/>
-      <c r="BL4" s="10"/>
-      <c r="BM4" s="10"/>
-      <c r="BN4" s="10"/>
-      <c r="BO4" s="10"/>
-      <c r="BP4" s="10"/>
-      <c r="BQ4" s="11"/>
+      <c r="BB4" s="14"/>
+      <c r="BC4" s="14"/>
+      <c r="BD4" s="14"/>
+      <c r="BE4" s="14"/>
+      <c r="BF4" s="14"/>
+      <c r="BG4" s="14"/>
+      <c r="BH4" s="14"/>
+      <c r="BI4" s="14"/>
+      <c r="BJ4" s="14"/>
+      <c r="BK4" s="14"/>
+      <c r="BL4" s="14"/>
+      <c r="BM4" s="14"/>
+      <c r="BN4" s="14"/>
+      <c r="BO4" s="14"/>
+      <c r="BP4" s="14"/>
+      <c r="BQ4" s="15"/>
       <c r="BR4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="BS4" s="10"/>
-      <c r="BT4" s="10"/>
-      <c r="BU4" s="10"/>
-      <c r="BV4" s="10"/>
-      <c r="BW4" s="10"/>
-      <c r="BX4" s="10"/>
-      <c r="BY4" s="10"/>
-      <c r="BZ4" s="10"/>
-      <c r="CA4" s="10"/>
-      <c r="CB4" s="10"/>
-      <c r="CC4" s="10"/>
-      <c r="CD4" s="10"/>
-      <c r="CE4" s="10"/>
-      <c r="CF4" s="10"/>
-      <c r="CG4" s="10"/>
-      <c r="CH4" s="10"/>
-      <c r="CI4" s="10"/>
-      <c r="CJ4" s="10"/>
-      <c r="CK4" s="10"/>
-      <c r="CL4" s="10"/>
-      <c r="CM4" s="10"/>
-      <c r="CN4" s="10"/>
-      <c r="CO4" s="10"/>
-      <c r="CP4" s="10"/>
-      <c r="CQ4" s="11"/>
+      <c r="BS4" s="14"/>
+      <c r="BT4" s="14"/>
+      <c r="BU4" s="14"/>
+      <c r="BV4" s="14"/>
+      <c r="BW4" s="14"/>
+      <c r="BX4" s="14"/>
+      <c r="BY4" s="14"/>
+      <c r="BZ4" s="14"/>
+      <c r="CA4" s="14"/>
+      <c r="CB4" s="14"/>
+      <c r="CC4" s="14"/>
+      <c r="CD4" s="14"/>
+      <c r="CE4" s="14"/>
+      <c r="CF4" s="14"/>
+      <c r="CG4" s="14"/>
+      <c r="CH4" s="14"/>
+      <c r="CI4" s="14"/>
+      <c r="CJ4" s="14"/>
+      <c r="CK4" s="14"/>
+      <c r="CL4" s="14"/>
+      <c r="CM4" s="14"/>
+      <c r="CN4" s="14"/>
+      <c r="CO4" s="14"/>
+      <c r="CP4" s="14"/>
+      <c r="CQ4" s="15"/>
       <c r="CR4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="CS4" s="10"/>
-      <c r="CT4" s="10"/>
-      <c r="CU4" s="10"/>
-      <c r="CV4" s="11"/>
+      <c r="CS4" s="14"/>
+      <c r="CT4" s="14"/>
+      <c r="CU4" s="14"/>
+      <c r="CV4" s="15"/>
       <c r="CW4" s="9" t="s">
         <v>17</v>
       </c>
@@ -1254,161 +1251,161 @@
       </c>
     </row>
     <row r="5" spans="1:103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="11"/>
+      <c r="Q5" s="15"/>
       <c r="R5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="10"/>
-      <c r="T5" s="11"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="15"/>
       <c r="U5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V5" s="10"/>
-      <c r="W5" s="11"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="15"/>
       <c r="X5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="11"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="15"/>
       <c r="AA5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="11"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="15"/>
       <c r="AD5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="11"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="15"/>
       <c r="AG5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AH5" s="11"/>
+      <c r="AH5" s="15"/>
       <c r="AI5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="11"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="15"/>
       <c r="AL5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AM5" s="10"/>
-      <c r="AN5" s="11"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="15"/>
       <c r="AO5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AP5" s="10"/>
-      <c r="AQ5" s="11"/>
+      <c r="AP5" s="14"/>
+      <c r="AQ5" s="15"/>
       <c r="AR5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AS5" s="10"/>
-      <c r="AT5" s="11"/>
+      <c r="AS5" s="14"/>
+      <c r="AT5" s="15"/>
       <c r="AU5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AV5" s="10"/>
-      <c r="AW5" s="11"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="15"/>
       <c r="AX5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AY5" s="10"/>
-      <c r="AZ5" s="11"/>
+      <c r="AY5" s="14"/>
+      <c r="AZ5" s="15"/>
       <c r="BA5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="BB5" s="11"/>
+      <c r="BB5" s="15"/>
       <c r="BC5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="BD5" s="10"/>
-      <c r="BE5" s="11"/>
+      <c r="BD5" s="14"/>
+      <c r="BE5" s="15"/>
       <c r="BF5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="BG5" s="10"/>
-      <c r="BH5" s="11"/>
+      <c r="BG5" s="14"/>
+      <c r="BH5" s="15"/>
       <c r="BI5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="BJ5" s="10"/>
-      <c r="BK5" s="11"/>
+      <c r="BJ5" s="14"/>
+      <c r="BK5" s="15"/>
       <c r="BL5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="BM5" s="10"/>
-      <c r="BN5" s="11"/>
+      <c r="BM5" s="14"/>
+      <c r="BN5" s="15"/>
       <c r="BO5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="BP5" s="10"/>
-      <c r="BQ5" s="11"/>
+      <c r="BP5" s="14"/>
+      <c r="BQ5" s="15"/>
       <c r="BR5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="BS5" s="11"/>
+      <c r="BS5" s="15"/>
       <c r="BT5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="BU5" s="10"/>
-      <c r="BV5" s="11"/>
+      <c r="BU5" s="14"/>
+      <c r="BV5" s="15"/>
       <c r="BW5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="BX5" s="10"/>
-      <c r="BY5" s="11"/>
+      <c r="BX5" s="14"/>
+      <c r="BY5" s="15"/>
       <c r="BZ5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="CA5" s="10"/>
-      <c r="CB5" s="11"/>
+      <c r="CA5" s="14"/>
+      <c r="CB5" s="15"/>
       <c r="CC5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="CD5" s="10"/>
-      <c r="CE5" s="11"/>
+      <c r="CD5" s="14"/>
+      <c r="CE5" s="15"/>
       <c r="CF5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="CG5" s="10"/>
-      <c r="CH5" s="11"/>
+      <c r="CG5" s="14"/>
+      <c r="CH5" s="15"/>
       <c r="CI5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="CJ5" s="10"/>
-      <c r="CK5" s="11"/>
+      <c r="CJ5" s="14"/>
+      <c r="CK5" s="15"/>
       <c r="CL5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="CM5" s="10"/>
-      <c r="CN5" s="11"/>
+      <c r="CM5" s="14"/>
+      <c r="CN5" s="15"/>
       <c r="CO5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="CP5" s="10"/>
-      <c r="CQ5" s="11"/>
+      <c r="CP5" s="14"/>
+      <c r="CQ5" s="15"/>
       <c r="CR5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1424,9 +1421,9 @@
       <c r="CV5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="CW5" s="12"/>
-      <c r="CX5" s="12"/>
-      <c r="CY5" s="12"/>
+      <c r="CW5" s="10"/>
+      <c r="CX5" s="10"/>
+      <c r="CY5" s="10"/>
     </row>
     <row r="6" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -1717,8 +1714,8 @@
       <c r="C7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>69</v>
+      <c r="D7" s="3">
+        <v>502533504</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>54</v>
@@ -1972,8 +1969,8 @@
       <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>69</v>
+      <c r="D8" s="3">
+        <v>502659064</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>54</v>
@@ -2211,7 +2208,7 @@
         <v>3660.63</v>
       </c>
       <c r="CX8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="CY8" s="3" t="s">
         <v>57</v>
@@ -2227,8 +2224,8 @@
       <c r="C9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>69</v>
+      <c r="D9" s="3">
+        <v>502659064</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>54</v>
@@ -2466,7 +2463,7 @@
         <v>3660.63</v>
       </c>
       <c r="CX9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CY9" s="3" t="s">
         <v>57</v>
@@ -2482,8 +2479,8 @@
       <c r="C10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>69</v>
+      <c r="D10" s="3">
+        <v>502533504</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>54</v>
@@ -2721,7 +2718,7 @@
         <v>3660.63</v>
       </c>
       <c r="CX10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="CY10" s="3" t="s">
         <v>57</v>
@@ -4620,29 +4617,12 @@
     <row r="29" spans="1:103" ht="63.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="BR4:CQ4"/>
-    <mergeCell ref="CR4:CV4"/>
-    <mergeCell ref="CW4:CW5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AK5"/>
-    <mergeCell ref="AL5:AN5"/>
-    <mergeCell ref="AO5:AQ5"/>
+    <mergeCell ref="CL5:CN5"/>
+    <mergeCell ref="CO5:CQ5"/>
+    <mergeCell ref="BR5:BS5"/>
+    <mergeCell ref="BT5:BV5"/>
+    <mergeCell ref="BW5:BY5"/>
+    <mergeCell ref="BZ5:CB5"/>
     <mergeCell ref="CX4:CX5"/>
     <mergeCell ref="CY4:CY5"/>
     <mergeCell ref="K5:L5"/>
@@ -4659,18 +4639,35 @@
     <mergeCell ref="AU5:AW5"/>
     <mergeCell ref="AX5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BR4:CQ4"/>
+    <mergeCell ref="CR4:CV4"/>
+    <mergeCell ref="CW4:CW5"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AK5"/>
+    <mergeCell ref="AL5:AN5"/>
+    <mergeCell ref="AO5:AQ5"/>
     <mergeCell ref="BC5:BE5"/>
     <mergeCell ref="BF5:BH5"/>
     <mergeCell ref="BI5:BK5"/>
     <mergeCell ref="BL5:BN5"/>
     <mergeCell ref="BO5:BQ5"/>
     <mergeCell ref="CI5:CK5"/>
-    <mergeCell ref="CL5:CN5"/>
-    <mergeCell ref="CO5:CQ5"/>
-    <mergeCell ref="BR5:BS5"/>
-    <mergeCell ref="BT5:BV5"/>
-    <mergeCell ref="BW5:BY5"/>
-    <mergeCell ref="BZ5:CB5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.78740157480314965" footer="0.78740157480314965"/>

</xml_diff>

<commit_message>
Pushing changes made last week. Added a loop surrounding the file prompt and default values for the questions to make the program less error prone.
</commit_message>
<xml_diff>
--- a/Top20Test.xlsx
+++ b/Top20Test.xlsx
@@ -459,6 +459,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -472,14 +480,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -982,7 +982,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1137,109 +1137,109 @@
       <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="15"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
       <c r="P4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="15"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="11"/>
       <c r="AG4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="14"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="14"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="14"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="14"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="14"/>
-      <c r="AY4" s="14"/>
-      <c r="AZ4" s="15"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="10"/>
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="10"/>
+      <c r="AP4" s="10"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
+      <c r="AV4" s="10"/>
+      <c r="AW4" s="10"/>
+      <c r="AX4" s="10"/>
+      <c r="AY4" s="10"/>
+      <c r="AZ4" s="11"/>
       <c r="BA4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BB4" s="14"/>
-      <c r="BC4" s="14"/>
-      <c r="BD4" s="14"/>
-      <c r="BE4" s="14"/>
-      <c r="BF4" s="14"/>
-      <c r="BG4" s="14"/>
-      <c r="BH4" s="14"/>
-      <c r="BI4" s="14"/>
-      <c r="BJ4" s="14"/>
-      <c r="BK4" s="14"/>
-      <c r="BL4" s="14"/>
-      <c r="BM4" s="14"/>
-      <c r="BN4" s="14"/>
-      <c r="BO4" s="14"/>
-      <c r="BP4" s="14"/>
-      <c r="BQ4" s="15"/>
+      <c r="BB4" s="10"/>
+      <c r="BC4" s="10"/>
+      <c r="BD4" s="10"/>
+      <c r="BE4" s="10"/>
+      <c r="BF4" s="10"/>
+      <c r="BG4" s="10"/>
+      <c r="BH4" s="10"/>
+      <c r="BI4" s="10"/>
+      <c r="BJ4" s="10"/>
+      <c r="BK4" s="10"/>
+      <c r="BL4" s="10"/>
+      <c r="BM4" s="10"/>
+      <c r="BN4" s="10"/>
+      <c r="BO4" s="10"/>
+      <c r="BP4" s="10"/>
+      <c r="BQ4" s="11"/>
       <c r="BR4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="BS4" s="14"/>
-      <c r="BT4" s="14"/>
-      <c r="BU4" s="14"/>
-      <c r="BV4" s="14"/>
-      <c r="BW4" s="14"/>
-      <c r="BX4" s="14"/>
-      <c r="BY4" s="14"/>
-      <c r="BZ4" s="14"/>
-      <c r="CA4" s="14"/>
-      <c r="CB4" s="14"/>
-      <c r="CC4" s="14"/>
-      <c r="CD4" s="14"/>
-      <c r="CE4" s="14"/>
-      <c r="CF4" s="14"/>
-      <c r="CG4" s="14"/>
-      <c r="CH4" s="14"/>
-      <c r="CI4" s="14"/>
-      <c r="CJ4" s="14"/>
-      <c r="CK4" s="14"/>
-      <c r="CL4" s="14"/>
-      <c r="CM4" s="14"/>
-      <c r="CN4" s="14"/>
-      <c r="CO4" s="14"/>
-      <c r="CP4" s="14"/>
-      <c r="CQ4" s="15"/>
+      <c r="BS4" s="10"/>
+      <c r="BT4" s="10"/>
+      <c r="BU4" s="10"/>
+      <c r="BV4" s="10"/>
+      <c r="BW4" s="10"/>
+      <c r="BX4" s="10"/>
+      <c r="BY4" s="10"/>
+      <c r="BZ4" s="10"/>
+      <c r="CA4" s="10"/>
+      <c r="CB4" s="10"/>
+      <c r="CC4" s="10"/>
+      <c r="CD4" s="10"/>
+      <c r="CE4" s="10"/>
+      <c r="CF4" s="10"/>
+      <c r="CG4" s="10"/>
+      <c r="CH4" s="10"/>
+      <c r="CI4" s="10"/>
+      <c r="CJ4" s="10"/>
+      <c r="CK4" s="10"/>
+      <c r="CL4" s="10"/>
+      <c r="CM4" s="10"/>
+      <c r="CN4" s="10"/>
+      <c r="CO4" s="10"/>
+      <c r="CP4" s="10"/>
+      <c r="CQ4" s="11"/>
       <c r="CR4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="CS4" s="14"/>
-      <c r="CT4" s="14"/>
-      <c r="CU4" s="14"/>
-      <c r="CV4" s="15"/>
+      <c r="CS4" s="10"/>
+      <c r="CT4" s="10"/>
+      <c r="CU4" s="10"/>
+      <c r="CV4" s="11"/>
       <c r="CW4" s="9" t="s">
         <v>17</v>
       </c>
@@ -1251,161 +1251,161 @@
       </c>
     </row>
     <row r="5" spans="1:103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="15"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="11"/>
       <c r="P5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="15"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="14"/>
-      <c r="T5" s="15"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="11"/>
       <c r="U5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V5" s="14"/>
-      <c r="W5" s="15"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="11"/>
       <c r="X5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="15"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="11"/>
       <c r="AA5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="15"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="11"/>
       <c r="AD5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="15"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="11"/>
       <c r="AG5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AH5" s="15"/>
+      <c r="AH5" s="11"/>
       <c r="AI5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="15"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="11"/>
       <c r="AL5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="15"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="11"/>
       <c r="AO5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AP5" s="14"/>
-      <c r="AQ5" s="15"/>
+      <c r="AP5" s="10"/>
+      <c r="AQ5" s="11"/>
       <c r="AR5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="15"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="11"/>
       <c r="AU5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="15"/>
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="11"/>
       <c r="AX5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="15"/>
+      <c r="AY5" s="10"/>
+      <c r="AZ5" s="11"/>
       <c r="BA5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="BB5" s="15"/>
+      <c r="BB5" s="11"/>
       <c r="BC5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="BD5" s="14"/>
-      <c r="BE5" s="15"/>
+      <c r="BD5" s="10"/>
+      <c r="BE5" s="11"/>
       <c r="BF5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="BG5" s="14"/>
-      <c r="BH5" s="15"/>
+      <c r="BG5" s="10"/>
+      <c r="BH5" s="11"/>
       <c r="BI5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="BJ5" s="14"/>
-      <c r="BK5" s="15"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="11"/>
       <c r="BL5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="BM5" s="14"/>
-      <c r="BN5" s="15"/>
+      <c r="BM5" s="10"/>
+      <c r="BN5" s="11"/>
       <c r="BO5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="BP5" s="14"/>
-      <c r="BQ5" s="15"/>
+      <c r="BP5" s="10"/>
+      <c r="BQ5" s="11"/>
       <c r="BR5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="BS5" s="15"/>
+      <c r="BS5" s="11"/>
       <c r="BT5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="BU5" s="14"/>
-      <c r="BV5" s="15"/>
+      <c r="BU5" s="10"/>
+      <c r="BV5" s="11"/>
       <c r="BW5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="BX5" s="14"/>
-      <c r="BY5" s="15"/>
+      <c r="BX5" s="10"/>
+      <c r="BY5" s="11"/>
       <c r="BZ5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="CA5" s="14"/>
-      <c r="CB5" s="15"/>
+      <c r="CA5" s="10"/>
+      <c r="CB5" s="11"/>
       <c r="CC5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="CD5" s="14"/>
-      <c r="CE5" s="15"/>
+      <c r="CD5" s="10"/>
+      <c r="CE5" s="11"/>
       <c r="CF5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="CG5" s="14"/>
-      <c r="CH5" s="15"/>
+      <c r="CG5" s="10"/>
+      <c r="CH5" s="11"/>
       <c r="CI5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="CJ5" s="14"/>
-      <c r="CK5" s="15"/>
+      <c r="CJ5" s="10"/>
+      <c r="CK5" s="11"/>
       <c r="CL5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="CM5" s="14"/>
-      <c r="CN5" s="15"/>
+      <c r="CM5" s="10"/>
+      <c r="CN5" s="11"/>
       <c r="CO5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="CP5" s="14"/>
-      <c r="CQ5" s="15"/>
+      <c r="CP5" s="10"/>
+      <c r="CQ5" s="11"/>
       <c r="CR5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1421,9 +1421,9 @@
       <c r="CV5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="CW5" s="10"/>
-      <c r="CX5" s="10"/>
-      <c r="CY5" s="10"/>
+      <c r="CW5" s="12"/>
+      <c r="CX5" s="12"/>
+      <c r="CY5" s="12"/>
     </row>
     <row r="6" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -1715,7 +1715,7 @@
         <v>65</v>
       </c>
       <c r="D7" s="3">
-        <v>502533504</v>
+        <v>502659064</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>54</v>
@@ -1969,9 +1969,7 @@
       <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="3">
-        <v>502659064</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
         <v>54</v>
       </c>
@@ -2224,9 +2222,7 @@
       <c r="C9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="3">
-        <v>502659064</v>
-      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
         <v>54</v>
       </c>
@@ -2479,9 +2475,7 @@
       <c r="C10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="3">
-        <v>502533504</v>
-      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>54</v>
       </c>
@@ -4617,12 +4611,35 @@
     <row r="29" spans="1:103" ht="63.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="CL5:CN5"/>
-    <mergeCell ref="CO5:CQ5"/>
-    <mergeCell ref="BR5:BS5"/>
-    <mergeCell ref="BT5:BV5"/>
-    <mergeCell ref="BW5:BY5"/>
-    <mergeCell ref="BZ5:CB5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="BR4:CQ4"/>
+    <mergeCell ref="CR4:CV4"/>
+    <mergeCell ref="CW4:CW5"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AK5"/>
+    <mergeCell ref="AL5:AN5"/>
+    <mergeCell ref="AO5:AQ5"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BL5:BN5"/>
+    <mergeCell ref="BO5:BQ5"/>
+    <mergeCell ref="CI5:CK5"/>
     <mergeCell ref="CX4:CX5"/>
     <mergeCell ref="CY4:CY5"/>
     <mergeCell ref="K5:L5"/>
@@ -4639,35 +4656,12 @@
     <mergeCell ref="AU5:AW5"/>
     <mergeCell ref="AX5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BR4:CQ4"/>
-    <mergeCell ref="CR4:CV4"/>
-    <mergeCell ref="CW4:CW5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AK5"/>
-    <mergeCell ref="AL5:AN5"/>
-    <mergeCell ref="AO5:AQ5"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="BF5:BH5"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="BL5:BN5"/>
-    <mergeCell ref="BO5:BQ5"/>
-    <mergeCell ref="CI5:CK5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="CL5:CN5"/>
+    <mergeCell ref="CO5:CQ5"/>
+    <mergeCell ref="BR5:BS5"/>
+    <mergeCell ref="BT5:BV5"/>
+    <mergeCell ref="BW5:BY5"/>
+    <mergeCell ref="BZ5:CB5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.78740157480314965" footer="0.78740157480314965"/>

</xml_diff>

<commit_message>
Updated template text, added Name, added separator, added signature line
</commit_message>
<xml_diff>
--- a/Top20Test.xlsx
+++ b/Top20Test.xlsx
@@ -212,9 +212,6 @@
     <t>phone4</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
     <t>user2</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>522639470</t>
+  </si>
+  <si>
+    <t>ZAIN NASRULLAH</t>
   </si>
 </sst>
 </file>
@@ -982,7 +982,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1712,7 +1712,7 @@
         <v>61</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3">
         <v>502659064</v>
@@ -1967,7 +1967,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
@@ -2206,7 +2206,7 @@
         <v>3660.63</v>
       </c>
       <c r="CX8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CY8" s="3" t="s">
         <v>57</v>
@@ -2220,7 +2220,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
@@ -2459,7 +2459,7 @@
         <v>3660.63</v>
       </c>
       <c r="CX9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="CY9" s="3" t="s">
         <v>57</v>
@@ -2473,7 +2473,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
@@ -2712,7 +2712,7 @@
         <v>3660.63</v>
       </c>
       <c r="CX10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CY10" s="3" t="s">
         <v>57</v>

</xml_diff>